<commit_message>
Updating the test data files
</commit_message>
<xml_diff>
--- a/Testdata/ManagePopulationsPage_Data.xlsx
+++ b/Testdata/ManagePopulationsPage_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VersionControl\pse.autotest\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF9362F-AD9B-4577-9000-14609EA44C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA79912-B69E-4033-9F98-145D71792113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{4E4E9E4E-34CE-4B5C-BC3C-B08A05AB3BC9}"/>
   </bookViews>
@@ -43,24 +43,6 @@
     <t>manage_population_file_to_upload</t>
   </si>
   <si>
-    <t>sample_population_data_sheet.xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet.xlsx</t>
-  </si>
-  <si>
-    <t>sample_population_data_sheet - Copy (1).xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet - Copy (1).xlsx</t>
-  </si>
-  <si>
-    <t>sample_population_data_sheet - Copy (2).xlsx</t>
-  </si>
-  <si>
-    <t>D:\\VersionControl\\pse.autotest\\ExtractionTemplate\\sample_population_data_sheet - Copy (2).xlsx</t>
-  </si>
-  <si>
     <t>Add_population_field</t>
   </si>
   <si>
@@ -83,6 +65,24 @@
   </si>
   <si>
     <t>This population is being created by Script for validation</t>
+  </si>
+  <si>
+    <t>\ExtractionTemplate\ManagePopulations\extraction-template-12.xlsx</t>
+  </si>
+  <si>
+    <t>extraction-template-12.xlsx</t>
+  </si>
+  <si>
+    <t>\ExtractionTemplate\ManagePopulations\extraction-template-14.xlsx</t>
+  </si>
+  <si>
+    <t>extraction-template-14.xlsx</t>
+  </si>
+  <si>
+    <t>\ExtractionTemplate\ManagePopulations\extraction-template-17.xlsx</t>
+  </si>
+  <si>
+    <t>extraction-template-17.xlsx</t>
   </si>
 </sst>
 </file>
@@ -441,13 +441,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="86.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -460,52 +460,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>